<commit_message>
Modified test data to remove PHYS 1110
</commit_message>
<xml_diff>
--- a/test_data/checklist1.xlsx
+++ b/test_data/checklist1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aidan/Desktop/github-repos/ECE_Graduation_Validation/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D43197C-C515-0C48-A28A-023484379AA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F13674-0750-4B49-AC3A-1DD33E1F9B35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20740" xr2:uid="{CCDFA643-959F-9442-8EA0-FAAE03167BCD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="119">
   <si>
     <t>Last Name:</t>
   </si>
@@ -78,9 +78,6 @@
     <t>CHEM 2090</t>
   </si>
   <si>
-    <t>PHYS 1110</t>
-  </si>
-  <si>
     <t>ECE 2300</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
   </si>
   <si>
     <t>Phys. 1</t>
-  </si>
-  <si>
-    <t>Exp. Phys.</t>
   </si>
   <si>
     <t>Phys. 2</t>
@@ -824,73 +818,73 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1217,7 +1211,7 @@
   <dimension ref="A2:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1237,20 +1231,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="21">
-      <c r="A2" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="A2" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
     </row>
     <row r="3" spans="1:12" ht="22" thickBot="1">
       <c r="A3" s="2"/>
@@ -1267,72 +1261,72 @@
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="33"/>
+      <c r="B4" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="50"/>
       <c r="H4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="31"/>
+      <c r="I4" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="32"/>
     </row>
     <row r="5" spans="1:12" ht="20" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="30">
         <v>1234567</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="32"/>
       <c r="G5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="31"/>
+      <c r="H5" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="32"/>
     </row>
     <row r="7" spans="1:12" ht="20" thickBot="1">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
+      <c r="G7" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
     </row>
     <row r="8" spans="1:12" ht="21" thickTop="1" thickBot="1">
       <c r="A8" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>7</v>
@@ -1344,10 +1338,10 @@
         <v>6</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" s="26" t="s">
         <v>7</v>
@@ -1358,7 +1352,7 @@
     </row>
     <row r="9" spans="1:12" ht="17" thickTop="1">
       <c r="A9" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -1367,30 +1361,30 @@
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I9" s="3">
         <v>4</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>10</v>
@@ -1399,30 +1393,30 @@
         <v>4</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I10" s="4">
         <v>3</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
@@ -1431,30 +1425,30 @@
         <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I11" s="4">
         <v>4</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>12</v>
@@ -1463,62 +1457,62 @@
         <v>4</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12" s="4">
         <v>4</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="4">
         <v>4</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I13" s="4">
         <v>4</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="17" thickBot="1">
       <c r="A14" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>13</v>
@@ -1527,93 +1521,83 @@
         <v>4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I14" s="5">
         <v>4</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="17" thickTop="1">
       <c r="A15" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="4">
         <v>3</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="20" thickBot="1">
-      <c r="A16" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="8"/>
+      <c r="G16" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
     </row>
     <row r="17" spans="1:12" ht="21" thickTop="1" thickBot="1">
       <c r="A17" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="4">
         <v>4</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G17" s="25" t="s">
         <v>6</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J17" s="26" t="s">
         <v>7</v>
@@ -1622,194 +1606,194 @@
         <v>8</v>
       </c>
       <c r="L17" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="17" thickTop="1">
       <c r="A18" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4">
         <v>4</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I18" s="3">
         <v>3</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="4">
         <v>4</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I19" s="4">
         <v>3</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I20" s="4">
         <v>3</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="17" thickBot="1">
       <c r="A21" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I21" s="4">
         <v>3</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" thickTop="1">
       <c r="G22" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I22" s="4">
         <v>3</v>
       </c>
       <c r="J22" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="20" thickBot="1">
+      <c r="A23" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="G23" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="20" thickBot="1">
-      <c r="A23" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="G23" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="I23" s="4">
         <v>3</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="21" thickTop="1" thickBot="1">
@@ -1817,10 +1801,10 @@
         <v>6</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>7</v>
@@ -1829,244 +1813,244 @@
         <v>8</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I24" s="4">
         <v>3</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="17" thickTop="1">
       <c r="A25" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="3">
         <v>4</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I25" s="4">
         <v>3</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="4">
         <v>4</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I26" s="4">
         <v>4</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="4">
         <v>4</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I27" s="4">
         <v>4</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="4">
         <v>4</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I28" s="4">
         <v>4</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="17" thickBot="1">
       <c r="A29" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" s="5">
         <v>4</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I29" s="4">
         <v>3</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="17" thickTop="1">
       <c r="G30" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I30" s="4">
         <v>3</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="20" thickBot="1">
-      <c r="A31" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
+      <c r="A31" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
       <c r="G31" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I31" s="4">
         <v>4</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="21" thickTop="1" thickBot="1">
@@ -2074,10 +2058,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>7</v>
@@ -2086,83 +2070,83 @@
         <v>8</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I32" s="5">
         <v>3</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="17" customHeight="1" thickTop="1" thickBot="1">
       <c r="A33" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C33" s="3">
         <v>2</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="16" customHeight="1" thickBot="1">
       <c r="A34" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C34" s="4">
         <v>3</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="H34" s="45"/>
-      <c r="I34" s="45"/>
-      <c r="J34" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="K34" s="47"/>
+        <v>75</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="K34" s="35"/>
       <c r="L34" s="17"/>
     </row>
     <row r="35" spans="1:13" ht="17" thickBot="1">
       <c r="A35" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C35" s="5">
         <v>1</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
@@ -2177,14 +2161,14 @@
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
-      <c r="G36" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
+      <c r="G36" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="48"/>
+      <c r="L36" s="48"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="24"/>
@@ -2192,97 +2176,97 @@
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
-      <c r="K37" s="42"/>
-      <c r="L37" s="42"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
     </row>
     <row r="38" spans="1:13" ht="17" thickBot="1">
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="42"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
+      <c r="L38" s="48"/>
     </row>
     <row r="39" spans="1:13" ht="21" thickTop="1" thickBot="1">
-      <c r="A39" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="41"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="42"/>
-      <c r="K39" s="42"/>
-      <c r="L39" s="42"/>
+      <c r="A39" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="47"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="48"/>
+      <c r="L39" s="48"/>
     </row>
     <row r="40" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A40" s="34" t="s">
+      <c r="A40" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="42"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="48"/>
+      <c r="L40" s="48"/>
+    </row>
+    <row r="41" spans="1:13" ht="18" thickTop="1" thickBot="1">
+      <c r="A41" s="40"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="44"/>
+    </row>
+    <row r="42" spans="1:13" ht="18" thickTop="1" thickBot="1">
+      <c r="A42" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="36"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
-      <c r="K40" s="42"/>
-      <c r="L40" s="42"/>
-    </row>
-    <row r="41" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A41" s="34"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="38"/>
-    </row>
-    <row r="42" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A42" s="43" t="s">
+      <c r="B42" s="36"/>
+      <c r="C42" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="31"/>
+      <c r="E42" s="32"/>
+      <c r="G42" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="K42" s="32"/>
+    </row>
+    <row r="43" spans="1:13" ht="18" thickTop="1" thickBot="1">
+      <c r="A43" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="48"/>
-      <c r="C42" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="30"/>
-      <c r="E42" s="31"/>
-      <c r="G42" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="K42" s="31"/>
-    </row>
-    <row r="43" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A43" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43" s="44"/>
-      <c r="C43" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="D43" s="30"/>
-      <c r="E43" s="31"/>
-      <c r="G43" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="50">
+      <c r="B43" s="29"/>
+      <c r="C43" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="31"/>
+      <c r="E43" s="32"/>
+      <c r="G43" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="38">
         <v>45269</v>
       </c>
-      <c r="K43" s="31"/>
+      <c r="K43" s="32"/>
     </row>
     <row r="44" spans="1:13" ht="17" thickTop="1"/>
     <row r="45" spans="1:13" ht="19">
@@ -3056,6 +3040,19 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="G16:L16"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="A40:E41"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="G36:L40"/>
+    <mergeCell ref="A31:E31"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="G34:I34"/>
@@ -3066,19 +3063,6 @@
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="G43:I43"/>
     <mergeCell ref="J43:K43"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="A40:E41"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="G36:L40"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="G16:L16"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="A7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated test data for correct credits
</commit_message>
<xml_diff>
--- a/test_data/checklist1.xlsx
+++ b/test_data/checklist1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aidan/Desktop/github-repos/ECE_Graduation_Validation/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F13674-0750-4B49-AC3A-1DD33E1F9B35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB95A9A-45CA-A245-B038-1A1323317040}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20740" xr2:uid="{CCDFA643-959F-9442-8EA0-FAAE03167BCD}"/>
   </bookViews>
@@ -818,21 +818,57 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -849,42 +885,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1211,7 +1211,7 @@
   <dimension ref="A2:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1231,20 +1231,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="21">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:12" ht="22" thickBot="1">
       <c r="A3" s="2"/>
@@ -1261,20 +1261,20 @@
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="50"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="33"/>
       <c r="H4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="32"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="31"/>
     </row>
     <row r="5" spans="1:12" ht="20" thickBot="1">
       <c r="A5" s="6" t="s">
@@ -1286,37 +1286,37 @@
       <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="29">
         <v>1234567</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="31"/>
       <c r="G5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="32"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="31"/>
     </row>
     <row r="7" spans="1:12" ht="20" thickBot="1">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:12" ht="21" thickTop="1" thickBot="1">
       <c r="A8" s="25" t="s">
@@ -1550,7 +1550,7 @@
         <v>67</v>
       </c>
       <c r="C15" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>74</v>
@@ -1565,14 +1565,14 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="8"/>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
     </row>
     <row r="17" spans="1:12" ht="21" thickTop="1" thickBot="1">
       <c r="A17" s="12" t="s">
@@ -1770,13 +1770,13 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="20" thickBot="1">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
       <c r="G23" s="12" t="s">
         <v>56</v>
       </c>
@@ -2027,13 +2027,13 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="20" thickBot="1">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
       <c r="G31" s="12" t="s">
         <v>59</v>
       </c>
@@ -2121,15 +2121,15 @@
       <c r="E34" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G34" s="33" t="s">
+      <c r="G34" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="34" t="s">
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="K34" s="35"/>
+      <c r="K34" s="47"/>
       <c r="L34" s="17"/>
     </row>
     <row r="35" spans="1:13" ht="17" thickBot="1">
@@ -2161,14 +2161,14 @@
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
-      <c r="G36" s="48" t="s">
+      <c r="G36" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="42"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="24"/>
@@ -2176,97 +2176,97 @@
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="42"/>
     </row>
     <row r="38" spans="1:13" ht="17" thickBot="1">
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="42"/>
     </row>
     <row r="39" spans="1:13" ht="21" thickTop="1" thickBot="1">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="47"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="48"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="41"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="42"/>
+      <c r="L39" s="42"/>
     </row>
     <row r="40" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="42"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="48"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="36"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
+      <c r="L40" s="42"/>
     </row>
     <row r="41" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A41" s="40"/>
-      <c r="B41" s="41"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="44"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="30" t="s">
+      <c r="B42" s="48"/>
+      <c r="C42" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="D42" s="31"/>
-      <c r="E42" s="32"/>
-      <c r="G42" s="37" t="s">
+      <c r="D42" s="30"/>
+      <c r="E42" s="31"/>
+      <c r="G42" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="30" t="s">
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="K42" s="32"/>
+      <c r="K42" s="31"/>
     </row>
     <row r="43" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="30" t="s">
+      <c r="B43" s="44"/>
+      <c r="C43" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D43" s="31"/>
-      <c r="E43" s="32"/>
-      <c r="G43" s="37" t="s">
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
+      <c r="G43" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="38">
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="50">
         <v>45269</v>
       </c>
-      <c r="K43" s="32"/>
+      <c r="K43" s="31"/>
     </row>
     <row r="44" spans="1:13" ht="17" thickTop="1"/>
     <row r="45" spans="1:13" ht="19">
@@ -3040,19 +3040,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="G16:L16"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="A40:E41"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="G36:L40"/>
-    <mergeCell ref="A31:E31"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="G34:I34"/>
@@ -3063,6 +3050,19 @@
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="G43:I43"/>
     <mergeCell ref="J43:K43"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="A40:E41"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="G36:L40"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="G16:L16"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="A7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>